<commit_message>
Remove sampleSizeValue in binary (xlsx) test data after rebasing
</commit_message>
<xml_diff>
--- a/scripts/processing/input/jane.doe@univ.se_210902-212121_ampliseq.xlsx
+++ b/scripts/processing/input/jane.doe@univ.se_210902-212121_ampliseq.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maria.prager/code/github/mol-mod/scripts/import-test/input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maria.prager/code/github/mol-mod/scripts/processing/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1FAE807-D361-F443-8C8D-56A01DE1F771}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0225BB24-FD7A-614E-8855-3F49C40E9F99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7360" yWindow="9760" windowWidth="38000" windowHeight="14600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7300" yWindow="1900" windowWidth="38000" windowHeight="14600" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="event" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="307">
   <si>
     <t>event_id_alias</t>
   </si>
@@ -1704,29 +1704,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AD991"/>
+  <dimension ref="A1:AC991"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="14.140625" style="6" customWidth="1"/>
     <col min="3" max="3" width="17" style="6" customWidth="1"/>
-    <col min="4" max="8" width="14.140625" style="6" customWidth="1"/>
-    <col min="9" max="9" width="18.85546875" style="6" customWidth="1"/>
-    <col min="10" max="10" width="23.28515625" style="6" customWidth="1"/>
-    <col min="11" max="14" width="14.140625" style="6" customWidth="1"/>
-    <col min="15" max="15" width="20.85546875" style="6" customWidth="1"/>
-    <col min="16" max="16" width="21.42578125" style="6" customWidth="1"/>
-    <col min="17" max="17" width="18.5703125" style="6" customWidth="1"/>
-    <col min="18" max="18" width="19" style="6" customWidth="1"/>
-    <col min="19" max="26" width="11.28515625" style="6" customWidth="1"/>
-    <col min="27" max="16384" width="11.28515625" style="6"/>
+    <col min="4" max="7" width="14.140625" style="6" customWidth="1"/>
+    <col min="8" max="8" width="18.85546875" style="6" customWidth="1"/>
+    <col min="9" max="9" width="23.28515625" style="6" customWidth="1"/>
+    <col min="10" max="13" width="14.140625" style="6" customWidth="1"/>
+    <col min="14" max="14" width="20.85546875" style="6" customWidth="1"/>
+    <col min="15" max="15" width="21.42578125" style="6" customWidth="1"/>
+    <col min="16" max="16" width="18.5703125" style="6" customWidth="1"/>
+    <col min="17" max="17" width="19" style="6" customWidth="1"/>
+    <col min="18" max="25" width="11.28515625" style="6" customWidth="1"/>
+    <col min="26" max="16384" width="11.28515625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1740,54 +1740,51 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="3" t="s">
         <v>17</v>
       </c>
+      <c r="R1" s="5"/>
       <c r="S1" s="5"/>
       <c r="T1" s="5"/>
       <c r="U1" s="5"/>
       <c r="V1" s="5"/>
-      <c r="W1" s="5"/>
-    </row>
-    <row r="2" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>199</v>
       </c>
@@ -1800,29 +1797,26 @@
       <c r="D2" s="15" t="s">
         <v>203</v>
       </c>
-      <c r="E2" s="6">
-        <v>5414</v>
+      <c r="F2" s="5">
+        <v>55.185000000000002</v>
       </c>
       <c r="G2" s="5">
-        <v>55.185000000000002</v>
-      </c>
-      <c r="H2" s="5">
         <v>13.791</v>
       </c>
-      <c r="I2" s="15" t="s">
+      <c r="H2" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="M2" s="5" t="s">
         <v>213</v>
+      </c>
+      <c r="P2" s="5">
+        <v>3</v>
       </c>
       <c r="Q2" s="5">
         <v>3</v>
       </c>
-      <c r="R2" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>198</v>
       </c>
@@ -1835,27 +1829,25 @@
       <c r="D3" s="15" t="s">
         <v>203</v>
       </c>
-      <c r="E3" s="6">
-        <v>37676</v>
+      <c r="F3" s="5">
+        <v>55.433999999999997</v>
       </c>
       <c r="G3" s="5">
-        <v>55.433999999999997</v>
-      </c>
-      <c r="H3" s="5">
         <v>14.813000000000001</v>
       </c>
-      <c r="I3" s="15" t="s">
+      <c r="H3" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="N3" s="5" t="s">
+      <c r="M3" s="5" t="s">
         <v>212</v>
+      </c>
+      <c r="P3" s="5">
+        <v>3</v>
       </c>
       <c r="Q3" s="5">
         <v>3</v>
       </c>
-      <c r="R3" s="5">
-        <v>3</v>
-      </c>
+      <c r="S3" s="5"/>
       <c r="T3" s="5"/>
       <c r="U3" s="5"/>
       <c r="V3" s="5"/>
@@ -1866,9 +1858,8 @@
       <c r="AA3" s="5"/>
       <c r="AB3" s="5"/>
       <c r="AC3" s="5"/>
-      <c r="AD3" s="5"/>
-    </row>
-    <row r="4" spans="1:30" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>197</v>
       </c>
@@ -1881,27 +1872,25 @@
       <c r="D4" s="15" t="s">
         <v>203</v>
       </c>
-      <c r="E4" s="6">
-        <v>41973</v>
+      <c r="F4" s="5">
+        <v>56.031999999999996</v>
       </c>
       <c r="G4" s="5">
-        <v>56.031999999999996</v>
-      </c>
-      <c r="H4" s="5">
         <v>16.649999999999999</v>
       </c>
-      <c r="I4" s="15" t="s">
+      <c r="H4" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="N4" s="5" t="s">
+      <c r="M4" s="5" t="s">
         <v>212</v>
+      </c>
+      <c r="P4" s="5">
+        <v>3</v>
       </c>
       <c r="Q4" s="5">
         <v>3</v>
       </c>
-      <c r="R4" s="5">
-        <v>3</v>
-      </c>
+      <c r="S4" s="5"/>
       <c r="T4" s="5"/>
       <c r="U4" s="5"/>
       <c r="V4" s="5"/>
@@ -1912,9 +1901,9 @@
       <c r="AA4" s="5"/>
       <c r="AB4" s="5"/>
       <c r="AC4" s="5"/>
-      <c r="AD4" s="5"/>
-    </row>
-    <row r="5" spans="1:30" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+      <c r="S5" s="5"/>
       <c r="T5" s="5"/>
       <c r="U5" s="5"/>
       <c r="V5" s="5"/>
@@ -1925,9 +1914,9 @@
       <c r="AA5" s="5"/>
       <c r="AB5" s="5"/>
       <c r="AC5" s="5"/>
-      <c r="AD5" s="5"/>
-    </row>
-    <row r="6" spans="1:30" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+      <c r="S6" s="5"/>
       <c r="T6" s="5"/>
       <c r="U6" s="5"/>
       <c r="V6" s="5"/>
@@ -1938,9 +1927,9 @@
       <c r="AA6" s="5"/>
       <c r="AB6" s="5"/>
       <c r="AC6" s="5"/>
-      <c r="AD6" s="5"/>
-    </row>
-    <row r="7" spans="1:30" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+      <c r="S7" s="5"/>
       <c r="T7" s="5"/>
       <c r="U7" s="5"/>
       <c r="V7" s="5"/>
@@ -1951,9 +1940,9 @@
       <c r="AA7" s="5"/>
       <c r="AB7" s="5"/>
       <c r="AC7" s="5"/>
-      <c r="AD7" s="5"/>
-    </row>
-    <row r="8" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S8" s="5"/>
       <c r="T8" s="5"/>
       <c r="U8" s="5"/>
       <c r="V8" s="5"/>
@@ -1964,9 +1953,9 @@
       <c r="AA8" s="5"/>
       <c r="AB8" s="5"/>
       <c r="AC8" s="5"/>
-      <c r="AD8" s="5"/>
-    </row>
-    <row r="9" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S9" s="5"/>
       <c r="T9" s="5"/>
       <c r="U9" s="5"/>
       <c r="V9" s="5"/>
@@ -1977,407 +1966,385 @@
       <c r="AA9" s="5"/>
       <c r="AB9" s="5"/>
       <c r="AC9" s="5"/>
-      <c r="AD9" s="5"/>
-    </row>
-    <row r="10" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C10" s="7"/>
     </row>
-    <row r="11" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C11" s="7"/>
     </row>
-    <row r="12" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C12" s="7"/>
     </row>
-    <row r="13" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C13" s="7"/>
     </row>
-    <row r="14" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="8"/>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
-      <c r="H14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="9"/>
       <c r="I14" s="9"/>
-      <c r="J14" s="9"/>
+      <c r="J14" s="8"/>
       <c r="K14" s="8"/>
-      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
       <c r="N14" s="8"/>
       <c r="O14" s="8"/>
       <c r="P14" s="8"/>
-      <c r="Q14" s="8"/>
-    </row>
-    <row r="15" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="10"/>
       <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="H15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="J15" s="5"/>
       <c r="K15" s="5"/>
-      <c r="L15" s="5"/>
-      <c r="M15" s="12"/>
-      <c r="N15" s="13"/>
+      <c r="L15" s="12"/>
+      <c r="M15" s="13"/>
+      <c r="N15" s="5"/>
       <c r="O15" s="5"/>
       <c r="P15" s="5"/>
-      <c r="Q15" s="5"/>
-    </row>
-    <row r="16" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="10"/>
       <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="H16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="J16" s="5"/>
       <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
-      <c r="M16" s="12"/>
-      <c r="N16" s="14"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="14"/>
+      <c r="N16" s="5"/>
       <c r="O16" s="5"/>
       <c r="P16" s="5"/>
-      <c r="Q16" s="5"/>
-    </row>
-    <row r="17" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="10"/>
       <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="H17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="J17" s="5"/>
       <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
-      <c r="M17" s="12"/>
-      <c r="N17" s="14"/>
+      <c r="L17" s="12"/>
+      <c r="M17" s="14"/>
+      <c r="N17" s="5"/>
       <c r="O17" s="5"/>
       <c r="P17" s="5"/>
-      <c r="Q17" s="5"/>
-    </row>
-    <row r="18" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="10"/>
       <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="H18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="J18" s="5"/>
       <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
-      <c r="M18" s="12"/>
-      <c r="N18" s="14"/>
+      <c r="L18" s="12"/>
+      <c r="M18" s="14"/>
+      <c r="N18" s="5"/>
       <c r="O18" s="5"/>
       <c r="P18" s="5"/>
-      <c r="Q18" s="5"/>
-    </row>
-    <row r="19" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
       <c r="D19" s="10"/>
       <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="H19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="J19" s="5"/>
       <c r="K19" s="5"/>
-      <c r="L19" s="5"/>
-      <c r="M19" s="12"/>
-      <c r="N19" s="14"/>
+      <c r="L19" s="12"/>
+      <c r="M19" s="14"/>
+      <c r="N19" s="5"/>
       <c r="O19" s="5"/>
       <c r="P19" s="5"/>
-      <c r="Q19" s="5"/>
-    </row>
-    <row r="20" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
       <c r="D20" s="10"/>
       <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="H20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="J20" s="5"/>
       <c r="K20" s="5"/>
-      <c r="L20" s="5"/>
-      <c r="M20" s="12"/>
-      <c r="N20" s="14"/>
+      <c r="L20" s="12"/>
+      <c r="M20" s="14"/>
+      <c r="N20" s="5"/>
       <c r="O20" s="5"/>
       <c r="P20" s="5"/>
-      <c r="Q20" s="5"/>
-    </row>
-    <row r="21" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
       <c r="D21" s="10"/>
       <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="H21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="J21" s="5"/>
       <c r="K21" s="5"/>
-      <c r="L21" s="5"/>
-      <c r="M21" s="12"/>
-      <c r="N21" s="14"/>
+      <c r="L21" s="12"/>
+      <c r="M21" s="14"/>
+      <c r="N21" s="5"/>
       <c r="O21" s="5"/>
       <c r="P21" s="5"/>
-      <c r="Q21" s="5"/>
-    </row>
-    <row r="22" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
       <c r="D22" s="10"/>
       <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="H22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="J22" s="5"/>
       <c r="K22" s="5"/>
-      <c r="L22" s="5"/>
-      <c r="M22" s="12"/>
-      <c r="N22" s="14"/>
+      <c r="L22" s="12"/>
+      <c r="M22" s="14"/>
+      <c r="N22" s="5"/>
       <c r="O22" s="5"/>
       <c r="P22" s="5"/>
-      <c r="Q22" s="5"/>
-    </row>
-    <row r="23" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="10"/>
       <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-      <c r="H23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="J23" s="5"/>
       <c r="K23" s="5"/>
-      <c r="L23" s="5"/>
-      <c r="M23" s="12"/>
-      <c r="N23" s="14"/>
+      <c r="L23" s="12"/>
+      <c r="M23" s="14"/>
+      <c r="N23" s="5"/>
       <c r="O23" s="5"/>
       <c r="P23" s="5"/>
-      <c r="Q23" s="5"/>
-    </row>
-    <row r="24" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="10"/>
       <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
-      <c r="H24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="J24" s="5"/>
       <c r="K24" s="5"/>
-      <c r="L24" s="5"/>
-      <c r="M24" s="12"/>
-      <c r="N24" s="14"/>
+      <c r="L24" s="12"/>
+      <c r="M24" s="14"/>
+      <c r="N24" s="5"/>
       <c r="O24" s="5"/>
       <c r="P24" s="5"/>
-      <c r="Q24" s="5"/>
-    </row>
-    <row r="25" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="10"/>
       <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
-      <c r="H25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="J25" s="5"/>
       <c r="K25" s="5"/>
-      <c r="L25" s="5"/>
-      <c r="M25" s="12"/>
-      <c r="N25" s="14"/>
+      <c r="L25" s="12"/>
+      <c r="M25" s="14"/>
+      <c r="N25" s="5"/>
       <c r="O25" s="5"/>
       <c r="P25" s="5"/>
-      <c r="Q25" s="5"/>
-    </row>
-    <row r="26" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="10"/>
       <c r="E26" s="11"/>
-      <c r="F26" s="11"/>
-      <c r="H26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="J26" s="5"/>
       <c r="K26" s="5"/>
-      <c r="L26" s="5"/>
-      <c r="M26" s="12"/>
-      <c r="N26" s="14"/>
+      <c r="L26" s="12"/>
+      <c r="M26" s="14"/>
+      <c r="N26" s="5"/>
       <c r="O26" s="5"/>
       <c r="P26" s="5"/>
-      <c r="Q26" s="5"/>
-    </row>
-    <row r="27" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="10"/>
       <c r="E27" s="11"/>
-      <c r="F27" s="11"/>
-      <c r="H27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="J27" s="5"/>
       <c r="K27" s="5"/>
-      <c r="L27" s="5"/>
-      <c r="M27" s="12"/>
-      <c r="N27" s="14"/>
+      <c r="L27" s="12"/>
+      <c r="M27" s="14"/>
+      <c r="N27" s="5"/>
       <c r="O27" s="5"/>
       <c r="P27" s="5"/>
-      <c r="Q27" s="5"/>
-    </row>
-    <row r="28" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="10"/>
       <c r="E28" s="11"/>
-      <c r="F28" s="11"/>
-      <c r="H28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="J28" s="5"/>
       <c r="K28" s="5"/>
-      <c r="L28" s="5"/>
-      <c r="M28" s="12"/>
-      <c r="N28" s="14"/>
+      <c r="L28" s="12"/>
+      <c r="M28" s="14"/>
+      <c r="N28" s="5"/>
       <c r="O28" s="5"/>
       <c r="P28" s="5"/>
-      <c r="Q28" s="5"/>
-    </row>
-    <row r="29" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="10"/>
       <c r="E29" s="11"/>
-      <c r="F29" s="11"/>
-      <c r="H29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="J29" s="5"/>
       <c r="K29" s="5"/>
-      <c r="L29" s="5"/>
-      <c r="M29" s="12"/>
-      <c r="N29" s="14"/>
+      <c r="L29" s="12"/>
+      <c r="M29" s="14"/>
+      <c r="N29" s="5"/>
       <c r="O29" s="5"/>
       <c r="P29" s="5"/>
-      <c r="Q29" s="5"/>
-    </row>
-    <row r="30" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="10"/>
       <c r="E30" s="11"/>
-      <c r="F30" s="11"/>
-      <c r="H30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="J30" s="5"/>
       <c r="K30" s="5"/>
-      <c r="L30" s="5"/>
-      <c r="M30" s="12"/>
-      <c r="N30" s="14"/>
+      <c r="L30" s="12"/>
+      <c r="M30" s="14"/>
+      <c r="N30" s="5"/>
       <c r="O30" s="5"/>
       <c r="P30" s="5"/>
-      <c r="Q30" s="5"/>
-    </row>
-    <row r="31" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="5"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
       <c r="D31" s="10"/>
       <c r="E31" s="11"/>
-      <c r="F31" s="11"/>
-      <c r="H31" s="5"/>
+      <c r="G31" s="5"/>
+      <c r="J31" s="5"/>
       <c r="K31" s="5"/>
-      <c r="L31" s="5"/>
-      <c r="M31" s="12"/>
-      <c r="N31" s="14"/>
+      <c r="L31" s="12"/>
+      <c r="M31" s="14"/>
+      <c r="N31" s="5"/>
       <c r="O31" s="5"/>
       <c r="P31" s="5"/>
-      <c r="Q31" s="5"/>
-    </row>
-    <row r="32" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="5"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="D32" s="10"/>
       <c r="E32" s="11"/>
-      <c r="F32" s="11"/>
-      <c r="H32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="J32" s="5"/>
       <c r="K32" s="5"/>
-      <c r="L32" s="5"/>
-      <c r="M32" s="12"/>
-      <c r="N32" s="14"/>
+      <c r="L32" s="12"/>
+      <c r="M32" s="14"/>
+      <c r="N32" s="5"/>
       <c r="O32" s="5"/>
       <c r="P32" s="5"/>
-      <c r="Q32" s="5"/>
-    </row>
-    <row r="33" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="5"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
       <c r="D33" s="10"/>
       <c r="E33" s="11"/>
-      <c r="F33" s="11"/>
-      <c r="H33" s="5"/>
+      <c r="G33" s="5"/>
+      <c r="J33" s="5"/>
       <c r="K33" s="5"/>
-      <c r="L33" s="5"/>
-      <c r="M33" s="12"/>
-      <c r="N33" s="14"/>
+      <c r="L33" s="12"/>
+      <c r="M33" s="14"/>
+      <c r="N33" s="5"/>
       <c r="O33" s="5"/>
       <c r="P33" s="5"/>
-      <c r="Q33" s="5"/>
-    </row>
-    <row r="34" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="5"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
       <c r="D34" s="10"/>
       <c r="E34" s="11"/>
-      <c r="F34" s="11"/>
-      <c r="H34" s="5"/>
+      <c r="G34" s="5"/>
+      <c r="J34" s="5"/>
       <c r="K34" s="5"/>
-      <c r="L34" s="5"/>
-      <c r="M34" s="12"/>
-      <c r="N34" s="14"/>
+      <c r="L34" s="12"/>
+      <c r="M34" s="14"/>
+      <c r="N34" s="5"/>
       <c r="O34" s="5"/>
       <c r="P34" s="5"/>
-      <c r="Q34" s="5"/>
-    </row>
-    <row r="35" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="5"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
       <c r="D35" s="10"/>
       <c r="E35" s="11"/>
-      <c r="F35" s="11"/>
-      <c r="H35" s="5"/>
+      <c r="G35" s="5"/>
+      <c r="J35" s="5"/>
       <c r="K35" s="5"/>
-      <c r="L35" s="5"/>
-      <c r="M35" s="12"/>
-      <c r="N35" s="14"/>
+      <c r="L35" s="12"/>
+      <c r="M35" s="14"/>
+      <c r="N35" s="5"/>
       <c r="O35" s="5"/>
       <c r="P35" s="5"/>
-      <c r="Q35" s="5"/>
-    </row>
-    <row r="36" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C36" s="7"/>
     </row>
-    <row r="37" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C37" s="7"/>
     </row>
-    <row r="38" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C38" s="7"/>
     </row>
-    <row r="39" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C39" s="7"/>
     </row>
-    <row r="40" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C40" s="7"/>
     </row>
-    <row r="41" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C41" s="7"/>
     </row>
-    <row r="42" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C42" s="7"/>
     </row>
-    <row r="43" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C43" s="7"/>
     </row>
-    <row r="44" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C44" s="7"/>
     </row>
-    <row r="45" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C45" s="7"/>
     </row>
-    <row r="46" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C46" s="7"/>
     </row>
-    <row r="47" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C47" s="7"/>
     </row>
-    <row r="48" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C48" s="7"/>
     </row>
     <row r="49" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5210,7 +5177,7 @@
       <c r="C991" s="7"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:V9">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:U9">
     <sortCondition ref="A3:A9"/>
   </sortState>
   <phoneticPr fontId="9" type="noConversion"/>
@@ -5223,7 +5190,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N977"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="H1" workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
@@ -9687,7 +9654,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{221FF7C6-E74E-E14F-A681-9750CC4E526F}">
   <dimension ref="A1:E973"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>

</xml_diff>